<commit_message>
merged branches and fixed save and load state
</commit_message>
<xml_diff>
--- a/module4/module4results.xlsx
+++ b/module4/module4results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="54">
   <si>
     <t>Learning rate0</t>
   </si>
@@ -233,12 +233,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,11 +256,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -273,12 +280,17 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,11 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1231"/>
+  <dimension ref="A1:I1366"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1208" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1226" sqref="A1226:A1231"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1294" sqref="G1294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,28 +642,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -28999,6 +29011,3123 @@
       </c>
       <c r="G1231" s="6">
         <v>77.6666666666666</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1232" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1232">
+        <v>0.5</v>
+      </c>
+      <c r="C1232" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1232">
+        <v>2</v>
+      </c>
+      <c r="E1232" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1232" s="6">
+        <v>81.25</v>
+      </c>
+      <c r="G1232" s="6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1233" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1233">
+        <v>0.5</v>
+      </c>
+      <c r="C1233" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1233">
+        <v>5</v>
+      </c>
+      <c r="E1233" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1233" s="6">
+        <v>79.25</v>
+      </c>
+      <c r="G1233" s="6">
+        <v>78.75</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1234" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1234">
+        <v>0.5</v>
+      </c>
+      <c r="C1234" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1234">
+        <v>8</v>
+      </c>
+      <c r="E1234" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1234" s="6">
+        <v>75.3125</v>
+      </c>
+      <c r="G1234" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1235" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1235">
+        <v>0.5</v>
+      </c>
+      <c r="C1235" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1235">
+        <v>2</v>
+      </c>
+      <c r="E1235" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1235" s="6">
+        <v>82.1875</v>
+      </c>
+      <c r="G1235" s="6">
+        <v>86.25</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1236" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1236">
+        <v>0.5</v>
+      </c>
+      <c r="C1236" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1236">
+        <v>5</v>
+      </c>
+      <c r="E1236" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1236" s="6">
+        <v>76.6875</v>
+      </c>
+      <c r="G1236" s="6">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1237" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1237">
+        <v>0.5</v>
+      </c>
+      <c r="C1237" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1237">
+        <v>8</v>
+      </c>
+      <c r="E1237" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1237" s="6">
+        <v>71.5</v>
+      </c>
+      <c r="G1237" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1238" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1238">
+        <v>0.6</v>
+      </c>
+      <c r="C1238" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1238">
+        <v>2</v>
+      </c>
+      <c r="E1238" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1238" s="6">
+        <v>80.25</v>
+      </c>
+      <c r="G1238" s="6">
+        <v>82.75</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1239" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1239">
+        <v>0.6</v>
+      </c>
+      <c r="C1239" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1239">
+        <v>5</v>
+      </c>
+      <c r="E1239" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1239" s="6">
+        <v>76.75</v>
+      </c>
+      <c r="G1239" s="6">
+        <v>78.75</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1240" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1240">
+        <v>0.6</v>
+      </c>
+      <c r="C1240" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1240">
+        <v>8</v>
+      </c>
+      <c r="E1240" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1240" s="6">
+        <v>75.8125</v>
+      </c>
+      <c r="G1240" s="6">
+        <v>75.25</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1241" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1241">
+        <v>0.6</v>
+      </c>
+      <c r="C1241" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1241">
+        <v>2</v>
+      </c>
+      <c r="E1241" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1241" s="6">
+        <v>82.0625</v>
+      </c>
+      <c r="G1241" s="6">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1242" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1242">
+        <v>0.6</v>
+      </c>
+      <c r="C1242" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1242">
+        <v>5</v>
+      </c>
+      <c r="E1242" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1242" s="6">
+        <v>76.1875</v>
+      </c>
+      <c r="G1242" s="6">
+        <v>73.25</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1243" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1243">
+        <v>0.6</v>
+      </c>
+      <c r="C1243" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1243">
+        <v>8</v>
+      </c>
+      <c r="E1243" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1243" s="6">
+        <v>71.9375</v>
+      </c>
+      <c r="G1243" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1244">
+        <v>6</v>
+      </c>
+      <c r="B1244">
+        <v>0.6</v>
+      </c>
+      <c r="C1244" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1244">
+        <v>2</v>
+      </c>
+      <c r="E1244" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1244" s="6">
+        <v>6010.2210298600003</v>
+      </c>
+      <c r="G1244" s="6">
+        <v>119270.589563</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1245" s="2">
+        <v>6</v>
+      </c>
+      <c r="B1245" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C1245" s="7">
+        <v>60000</v>
+      </c>
+      <c r="D1245" s="2">
+        <v>5</v>
+      </c>
+      <c r="E1245" s="7">
+        <v>25000</v>
+      </c>
+      <c r="F1245" s="7">
+        <v>6288.0847741199996</v>
+      </c>
+      <c r="G1245" s="7">
+        <v>114412.835913</v>
+      </c>
+      <c r="H1245" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1246">
+        <v>6</v>
+      </c>
+      <c r="B1246">
+        <v>0.6</v>
+      </c>
+      <c r="C1246" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1246">
+        <v>8</v>
+      </c>
+      <c r="E1246" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1246" s="6">
+        <v>9190.4553088899993</v>
+      </c>
+      <c r="G1246" s="6">
+        <v>117833.200776</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1247">
+        <v>6</v>
+      </c>
+      <c r="B1247">
+        <v>0.6</v>
+      </c>
+      <c r="C1247" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1247">
+        <v>11</v>
+      </c>
+      <c r="E1247" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1247" s="6">
+        <v>5180.3360384999996</v>
+      </c>
+      <c r="G1247" s="6">
+        <v>115184.20684499999</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1248">
+        <v>6</v>
+      </c>
+      <c r="B1248">
+        <v>0.6</v>
+      </c>
+      <c r="C1248" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1248">
+        <v>14</v>
+      </c>
+      <c r="E1248" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1248" s="6">
+        <v>8447.3875146800001</v>
+      </c>
+      <c r="G1248" s="6">
+        <v>115324.813899</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1249">
+        <v>6</v>
+      </c>
+      <c r="B1249">
+        <v>0.6</v>
+      </c>
+      <c r="C1249" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1249">
+        <v>2</v>
+      </c>
+      <c r="E1249" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1249" s="6">
+        <v>4844.0306508900003</v>
+      </c>
+      <c r="G1249" s="6">
+        <v>115883.972371</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1250">
+        <v>6</v>
+      </c>
+      <c r="B1250">
+        <v>0.6</v>
+      </c>
+      <c r="C1250" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1250">
+        <v>5</v>
+      </c>
+      <c r="E1250" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1250" s="6">
+        <v>5599.8744571500001</v>
+      </c>
+      <c r="G1250" s="6">
+        <v>113831.60363899999</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1251">
+        <v>6</v>
+      </c>
+      <c r="B1251">
+        <v>0.6</v>
+      </c>
+      <c r="C1251" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1251">
+        <v>8</v>
+      </c>
+      <c r="E1251" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1251" s="6">
+        <v>7506.1940843399998</v>
+      </c>
+      <c r="G1251" s="6">
+        <v>121088.94704699999</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1252">
+        <v>6</v>
+      </c>
+      <c r="B1252">
+        <v>0.6</v>
+      </c>
+      <c r="C1252" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1252">
+        <v>11</v>
+      </c>
+      <c r="E1252" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1252" s="6">
+        <v>6898.6925184499996</v>
+      </c>
+      <c r="G1252" s="6">
+        <v>116350.78053</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1253">
+        <v>6</v>
+      </c>
+      <c r="B1253">
+        <v>0.6</v>
+      </c>
+      <c r="C1253" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1253">
+        <v>14</v>
+      </c>
+      <c r="E1253" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1253" s="6">
+        <v>10202.7896791</v>
+      </c>
+      <c r="G1253" s="6">
+        <v>115213.644507</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1254">
+        <v>6</v>
+      </c>
+      <c r="B1254">
+        <v>0.7</v>
+      </c>
+      <c r="C1254" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1254">
+        <v>2</v>
+      </c>
+      <c r="E1254" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1254" s="6">
+        <v>7103.7998982899999</v>
+      </c>
+      <c r="G1254" s="6">
+        <v>118411.04178100001</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1255">
+        <v>6</v>
+      </c>
+      <c r="B1255">
+        <v>0.7</v>
+      </c>
+      <c r="C1255" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1255">
+        <v>5</v>
+      </c>
+      <c r="E1255" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1255" s="6">
+        <v>5947.7965603700004</v>
+      </c>
+      <c r="G1255" s="6">
+        <v>116701.459462</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1256">
+        <v>6</v>
+      </c>
+      <c r="B1256">
+        <v>0.7</v>
+      </c>
+      <c r="C1256" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1256">
+        <v>8</v>
+      </c>
+      <c r="E1256" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1256" s="6">
+        <v>7041.5197319400004</v>
+      </c>
+      <c r="G1256" s="6">
+        <v>115136.282486</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1257">
+        <v>6</v>
+      </c>
+      <c r="B1257">
+        <v>0.7</v>
+      </c>
+      <c r="C1257" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1257">
+        <v>11</v>
+      </c>
+      <c r="E1257" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1257" s="6">
+        <v>7052.2051287800005</v>
+      </c>
+      <c r="G1257" s="6">
+        <v>117379.89371999999</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1258">
+        <v>6</v>
+      </c>
+      <c r="B1258">
+        <v>0.7</v>
+      </c>
+      <c r="C1258" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1258">
+        <v>14</v>
+      </c>
+      <c r="E1258" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1258" s="6">
+        <v>10332.1971663</v>
+      </c>
+      <c r="G1258" s="6">
+        <v>117498.72667</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1259">
+        <v>6</v>
+      </c>
+      <c r="B1259">
+        <v>0.7</v>
+      </c>
+      <c r="C1259" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1259">
+        <v>2</v>
+      </c>
+      <c r="E1259" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1259" s="6">
+        <v>3994.0306508899998</v>
+      </c>
+      <c r="G1259" s="6">
+        <v>118103.02118900001</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1260">
+        <v>6</v>
+      </c>
+      <c r="B1260">
+        <v>0.7</v>
+      </c>
+      <c r="C1260" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1260">
+        <v>5</v>
+      </c>
+      <c r="E1260" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1260" s="6">
+        <v>5336.7166957099998</v>
+      </c>
+      <c r="G1260" s="6">
+        <v>116321.860587</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1261">
+        <v>6</v>
+      </c>
+      <c r="B1261">
+        <v>0.7</v>
+      </c>
+      <c r="C1261" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1261">
+        <v>8</v>
+      </c>
+      <c r="E1261" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1261" s="6">
+        <v>6515.9156174</v>
+      </c>
+      <c r="G1261" s="6">
+        <v>114207.76880599999</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1262">
+        <v>6</v>
+      </c>
+      <c r="B1262">
+        <v>0.7</v>
+      </c>
+      <c r="C1262" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1262">
+        <v>11</v>
+      </c>
+      <c r="E1262" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1262" s="6">
+        <v>6740.2466759299996</v>
+      </c>
+      <c r="G1262" s="6">
+        <v>115390.217252</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1263">
+        <v>6</v>
+      </c>
+      <c r="B1263">
+        <v>0.7</v>
+      </c>
+      <c r="C1263" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1263">
+        <v>14</v>
+      </c>
+      <c r="E1263" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1263" s="6">
+        <v>9987.6325464199999</v>
+      </c>
+      <c r="G1263" s="6">
+        <v>113539.35608699999</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1264">
+        <v>7</v>
+      </c>
+      <c r="B1264">
+        <v>0.6</v>
+      </c>
+      <c r="C1264" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1264">
+        <v>2</v>
+      </c>
+      <c r="E1264" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1264" s="6">
+        <v>3813.0908980700001</v>
+      </c>
+      <c r="G1264" s="6">
+        <v>64665.572301400003</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1265">
+        <v>7</v>
+      </c>
+      <c r="B1265">
+        <v>0.6</v>
+      </c>
+      <c r="C1265" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1265">
+        <v>5</v>
+      </c>
+      <c r="E1265" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1265" s="6">
+        <v>4010.45680021</v>
+      </c>
+      <c r="G1265" s="6">
+        <v>63796.858394700001</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1266">
+        <v>7</v>
+      </c>
+      <c r="B1266">
+        <v>0.6</v>
+      </c>
+      <c r="C1266" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1266">
+        <v>8</v>
+      </c>
+      <c r="E1266" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1266" s="6">
+        <v>3997.48190884</v>
+      </c>
+      <c r="G1266" s="6">
+        <v>62939.561622499998</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1267">
+        <v>7</v>
+      </c>
+      <c r="B1267">
+        <v>0.6</v>
+      </c>
+      <c r="C1267" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1267">
+        <v>11</v>
+      </c>
+      <c r="E1267" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1267" s="6">
+        <v>4726.0258607200003</v>
+      </c>
+      <c r="G1267" s="6">
+        <v>63918.185358900002</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1268">
+        <v>7</v>
+      </c>
+      <c r="B1268">
+        <v>0.6</v>
+      </c>
+      <c r="C1268" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1268">
+        <v>14</v>
+      </c>
+      <c r="E1268" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1268" s="6">
+        <v>6111.0998855899998</v>
+      </c>
+      <c r="G1268" s="6">
+        <v>65505.983580499997</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1269">
+        <v>7</v>
+      </c>
+      <c r="B1269">
+        <v>0.6</v>
+      </c>
+      <c r="C1269" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1269">
+        <v>2</v>
+      </c>
+      <c r="E1269" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1269" s="6">
+        <v>4132.3877120200004</v>
+      </c>
+      <c r="G1269" s="6">
+        <v>63341.158995600003</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1270">
+        <v>7</v>
+      </c>
+      <c r="B1270">
+        <v>0.6</v>
+      </c>
+      <c r="C1270" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1270">
+        <v>5</v>
+      </c>
+      <c r="E1270" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1270" s="6">
+        <v>3842.06906471</v>
+      </c>
+      <c r="G1270" s="6">
+        <v>63417.113184499998</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1271" s="2">
+        <v>7</v>
+      </c>
+      <c r="B1271" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C1271" s="7">
+        <v>80000</v>
+      </c>
+      <c r="D1271" s="2">
+        <v>8</v>
+      </c>
+      <c r="E1271" s="7">
+        <v>25000</v>
+      </c>
+      <c r="F1271" s="7">
+        <v>3289.8766697299998</v>
+      </c>
+      <c r="G1271" s="7">
+        <v>62713.338335300003</v>
+      </c>
+      <c r="H1271" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1272">
+        <v>7</v>
+      </c>
+      <c r="B1272">
+        <v>0.6</v>
+      </c>
+      <c r="C1272" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1272">
+        <v>11</v>
+      </c>
+      <c r="E1272" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1272" s="6">
+        <v>4211.86639165</v>
+      </c>
+      <c r="G1272" s="6">
+        <v>63757.958377000003</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1273">
+        <v>7</v>
+      </c>
+      <c r="B1273">
+        <v>0.6</v>
+      </c>
+      <c r="C1273" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1273">
+        <v>14</v>
+      </c>
+      <c r="E1273" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1273" s="6">
+        <v>4843.8533547400002</v>
+      </c>
+      <c r="G1273" s="6">
+        <v>62731.047752799997</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1274">
+        <v>7</v>
+      </c>
+      <c r="B1274">
+        <v>0.7</v>
+      </c>
+      <c r="C1274" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1274">
+        <v>2</v>
+      </c>
+      <c r="E1274" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1274" s="6">
+        <v>4246.77224931</v>
+      </c>
+      <c r="G1274" s="6">
+        <v>63407.519937899997</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1275">
+        <v>7</v>
+      </c>
+      <c r="B1275">
+        <v>0.7</v>
+      </c>
+      <c r="C1275" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1275">
+        <v>5</v>
+      </c>
+      <c r="E1275" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1275" s="6">
+        <v>3494.1381324700001</v>
+      </c>
+      <c r="G1275" s="6">
+        <v>61511.203539100003</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1276">
+        <v>7</v>
+      </c>
+      <c r="B1276">
+        <v>0.7</v>
+      </c>
+      <c r="C1276" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1276">
+        <v>8</v>
+      </c>
+      <c r="E1276" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1276" s="6">
+        <v>3890.7066658200001</v>
+      </c>
+      <c r="G1276" s="6">
+        <v>64403.443640500001</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1277">
+        <v>7</v>
+      </c>
+      <c r="B1277">
+        <v>0.7</v>
+      </c>
+      <c r="C1277" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1277">
+        <v>11</v>
+      </c>
+      <c r="E1277" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1277" s="6">
+        <v>4555.9112832700002</v>
+      </c>
+      <c r="G1277" s="6">
+        <v>62851.272349899999</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1278">
+        <v>7</v>
+      </c>
+      <c r="B1278">
+        <v>0.7</v>
+      </c>
+      <c r="C1278" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1278">
+        <v>14</v>
+      </c>
+      <c r="E1278" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1278" s="6">
+        <v>4879.4383822399996</v>
+      </c>
+      <c r="G1278" s="6">
+        <v>63543.095472499997</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1279">
+        <v>7</v>
+      </c>
+      <c r="B1279">
+        <v>0.7</v>
+      </c>
+      <c r="C1279" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1279">
+        <v>2</v>
+      </c>
+      <c r="E1279" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1279" s="6">
+        <v>3856.1381265199998</v>
+      </c>
+      <c r="G1279" s="6">
+        <v>64871.287708999997</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1280">
+        <v>7</v>
+      </c>
+      <c r="B1280">
+        <v>0.7</v>
+      </c>
+      <c r="C1280" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1280">
+        <v>5</v>
+      </c>
+      <c r="E1280" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1280" s="6">
+        <v>3091.03986545</v>
+      </c>
+      <c r="G1280" s="6">
+        <v>62379.362055099999</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1281">
+        <v>7</v>
+      </c>
+      <c r="B1281">
+        <v>0.7</v>
+      </c>
+      <c r="C1281" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1281">
+        <v>8</v>
+      </c>
+      <c r="E1281" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1281" s="6">
+        <v>3846.3411030799998</v>
+      </c>
+      <c r="G1281" s="6">
+        <v>64153.482776500001</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1282">
+        <v>7</v>
+      </c>
+      <c r="B1282">
+        <v>0.7</v>
+      </c>
+      <c r="C1282" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1282">
+        <v>11</v>
+      </c>
+      <c r="E1282" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1282" s="6">
+        <v>3928.6365524600001</v>
+      </c>
+      <c r="G1282" s="6">
+        <v>62714.657030199996</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1283">
+        <v>7</v>
+      </c>
+      <c r="B1283">
+        <v>0.7</v>
+      </c>
+      <c r="C1283" s="6">
+        <v>80000</v>
+      </c>
+      <c r="D1283">
+        <v>14</v>
+      </c>
+      <c r="E1283" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F1283" s="6">
+        <v>5871.78321899</v>
+      </c>
+      <c r="G1283" s="6">
+        <v>65661.4921283</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1284" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1284">
+        <v>0.5</v>
+      </c>
+      <c r="C1284" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1284">
+        <v>5</v>
+      </c>
+      <c r="E1284" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1284" s="6">
+        <v>85.75</v>
+      </c>
+      <c r="G1284" s="6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1285" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1285">
+        <v>0.5</v>
+      </c>
+      <c r="C1285" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1285">
+        <v>8</v>
+      </c>
+      <c r="E1285" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1285" s="6">
+        <v>84.25</v>
+      </c>
+      <c r="G1285" s="6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1286" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1286">
+        <v>0.5</v>
+      </c>
+      <c r="C1286" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1286">
+        <v>2</v>
+      </c>
+      <c r="E1286" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1286" s="6">
+        <v>89</v>
+      </c>
+      <c r="G1286" s="6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1287" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1287">
+        <v>0.5</v>
+      </c>
+      <c r="C1287" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1287">
+        <v>5</v>
+      </c>
+      <c r="E1287" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1287" s="6">
+        <v>85.75</v>
+      </c>
+      <c r="G1287" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1288" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1288">
+        <v>0.5</v>
+      </c>
+      <c r="C1288" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1288">
+        <v>8</v>
+      </c>
+      <c r="E1288" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1288" s="6">
+        <v>85.5</v>
+      </c>
+      <c r="G1288" s="6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1289" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1289" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C1289" s="7">
+        <v>30000</v>
+      </c>
+      <c r="D1289" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1289" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F1289" s="7">
+        <v>89.75</v>
+      </c>
+      <c r="G1289" s="7">
+        <v>83</v>
+      </c>
+      <c r="H1289" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1290" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1290">
+        <v>0.6</v>
+      </c>
+      <c r="C1290" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1290">
+        <v>5</v>
+      </c>
+      <c r="E1290" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1290" s="6">
+        <v>87.75</v>
+      </c>
+      <c r="G1290" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1291" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1291">
+        <v>0.6</v>
+      </c>
+      <c r="C1291" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D1291">
+        <v>8</v>
+      </c>
+      <c r="E1291" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1291" s="6">
+        <v>82.25</v>
+      </c>
+      <c r="G1291" s="6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1292" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1292" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C1292" s="7">
+        <v>40000</v>
+      </c>
+      <c r="D1292" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1292" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F1292" s="7">
+        <v>91.5</v>
+      </c>
+      <c r="G1292" s="7">
+        <v>87</v>
+      </c>
+      <c r="H1292" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1293" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1293">
+        <v>0.6</v>
+      </c>
+      <c r="C1293" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1293">
+        <v>5</v>
+      </c>
+      <c r="E1293" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1293" s="6">
+        <v>86.25</v>
+      </c>
+      <c r="G1293" s="6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1294" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1294">
+        <v>0.6</v>
+      </c>
+      <c r="C1294" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1294">
+        <v>8</v>
+      </c>
+      <c r="E1294" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1294" s="6">
+        <v>84.75</v>
+      </c>
+      <c r="G1294" s="6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1295" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1295">
+        <v>0.6</v>
+      </c>
+      <c r="C1295" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1295">
+        <v>2</v>
+      </c>
+      <c r="E1295" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1295" s="6">
+        <v>82.375</v>
+      </c>
+      <c r="G1295" s="6">
+        <v>81.899999999999906</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1296" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1296">
+        <v>0.6</v>
+      </c>
+      <c r="C1296" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1296">
+        <v>2</v>
+      </c>
+      <c r="E1296" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1296" s="6">
+        <v>81.8</v>
+      </c>
+      <c r="G1296" s="6">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1297" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1297">
+        <v>0.6</v>
+      </c>
+      <c r="C1297" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1297">
+        <v>5</v>
+      </c>
+      <c r="E1297" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1297" s="6">
+        <v>83.375</v>
+      </c>
+      <c r="G1297" s="6">
+        <v>81.899999999999906</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1298" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1298">
+        <v>0.6</v>
+      </c>
+      <c r="C1298" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1298">
+        <v>5</v>
+      </c>
+      <c r="E1298" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1298" s="6">
+        <v>75.224999999999994</v>
+      </c>
+      <c r="G1298" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1299" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1299">
+        <v>0.6</v>
+      </c>
+      <c r="C1299" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1299">
+        <v>8</v>
+      </c>
+      <c r="E1299" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1299" s="6">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="G1299" s="6">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1300" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1300">
+        <v>0.6</v>
+      </c>
+      <c r="C1300" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1300">
+        <v>8</v>
+      </c>
+      <c r="E1300" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1300" s="6">
+        <v>67.774999999999906</v>
+      </c>
+      <c r="G1300" s="6">
+        <v>66.3</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1301" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1301">
+        <v>0.6</v>
+      </c>
+      <c r="C1301" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1301">
+        <v>2</v>
+      </c>
+      <c r="E1301" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1301" s="6">
+        <v>82.8</v>
+      </c>
+      <c r="G1301" s="6">
+        <v>83.1</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1302" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1302">
+        <v>0.6</v>
+      </c>
+      <c r="C1302" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1302">
+        <v>2</v>
+      </c>
+      <c r="E1302" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1302" s="6">
+        <v>82.625</v>
+      </c>
+      <c r="G1302" s="6">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1303" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1303">
+        <v>0.6</v>
+      </c>
+      <c r="C1303" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1303">
+        <v>5</v>
+      </c>
+      <c r="E1303" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1303" s="6">
+        <v>82.45</v>
+      </c>
+      <c r="G1303" s="6">
+        <v>82.399999999999906</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1304" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1304">
+        <v>0.6</v>
+      </c>
+      <c r="C1304" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1304">
+        <v>5</v>
+      </c>
+      <c r="E1304" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1304" s="6">
+        <v>73.424999999999997</v>
+      </c>
+      <c r="G1304" s="6">
+        <v>73.900000000000006</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1305" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1305">
+        <v>0.6</v>
+      </c>
+      <c r="C1305" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1305">
+        <v>8</v>
+      </c>
+      <c r="E1305" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1305" s="6">
+        <v>81.025000000000006</v>
+      </c>
+      <c r="G1305" s="6">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1306" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1306">
+        <v>0.6</v>
+      </c>
+      <c r="C1306" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1306">
+        <v>8</v>
+      </c>
+      <c r="E1306" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1306" s="6">
+        <v>63.524999999999999</v>
+      </c>
+      <c r="G1306" s="6">
+        <v>60.9</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1307" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1307">
+        <v>0.6</v>
+      </c>
+      <c r="C1307" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1307">
+        <v>2</v>
+      </c>
+      <c r="E1307" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1307" s="6">
+        <v>79.724999999999994</v>
+      </c>
+      <c r="G1307" s="6">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1308" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1308">
+        <v>0.6</v>
+      </c>
+      <c r="C1308" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1308">
+        <v>2</v>
+      </c>
+      <c r="E1308" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1308" s="6">
+        <v>81.575000000000003</v>
+      </c>
+      <c r="G1308" s="6">
+        <v>81.3</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1309" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1309">
+        <v>0.6</v>
+      </c>
+      <c r="C1309" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1309">
+        <v>5</v>
+      </c>
+      <c r="E1309" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1309" s="6">
+        <v>81.625</v>
+      </c>
+      <c r="G1309" s="6">
+        <v>78.3</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1310" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1310">
+        <v>0.6</v>
+      </c>
+      <c r="C1310" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1310">
+        <v>5</v>
+      </c>
+      <c r="E1310" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1310" s="6">
+        <v>75.25</v>
+      </c>
+      <c r="G1310" s="6">
+        <v>74.8</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1311" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1311">
+        <v>0.6</v>
+      </c>
+      <c r="C1311" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1311">
+        <v>8</v>
+      </c>
+      <c r="E1311" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1311" s="6">
+        <v>80.55</v>
+      </c>
+      <c r="G1311" s="6">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1312" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1312">
+        <v>0.6</v>
+      </c>
+      <c r="C1312" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1312">
+        <v>8</v>
+      </c>
+      <c r="E1312" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1312" s="6">
+        <v>68.3</v>
+      </c>
+      <c r="G1312" s="6">
+        <v>68.3</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1313" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1313">
+        <v>0.6</v>
+      </c>
+      <c r="C1313" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1313">
+        <v>2</v>
+      </c>
+      <c r="E1313" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1313" s="6">
+        <v>80.724999999999994</v>
+      </c>
+      <c r="G1313" s="6">
+        <v>82.1</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1314" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1314">
+        <v>0.6</v>
+      </c>
+      <c r="C1314" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1314">
+        <v>2</v>
+      </c>
+      <c r="E1314" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1314" s="6">
+        <v>81.075000000000003</v>
+      </c>
+      <c r="G1314" s="6">
+        <v>80.3</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1315" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1315">
+        <v>0.6</v>
+      </c>
+      <c r="C1315" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1315">
+        <v>5</v>
+      </c>
+      <c r="E1315" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1315" s="6">
+        <v>79.55</v>
+      </c>
+      <c r="G1315" s="6">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1316" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1316">
+        <v>0.6</v>
+      </c>
+      <c r="C1316" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1316">
+        <v>5</v>
+      </c>
+      <c r="E1316" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1316" s="6">
+        <v>74.724999999999994</v>
+      </c>
+      <c r="G1316" s="6">
+        <v>73.599999999999994</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1317" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1317">
+        <v>0.6</v>
+      </c>
+      <c r="C1317" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1317">
+        <v>8</v>
+      </c>
+      <c r="E1317" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1317" s="6">
+        <v>80.474999999999994</v>
+      </c>
+      <c r="G1317" s="6">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1318" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1318">
+        <v>0.6</v>
+      </c>
+      <c r="C1318" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1318">
+        <v>8</v>
+      </c>
+      <c r="E1318" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1318" s="6">
+        <v>65.025000000000006</v>
+      </c>
+      <c r="G1318" s="6">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1319" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1319">
+        <v>0.7</v>
+      </c>
+      <c r="C1319" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1319">
+        <v>2</v>
+      </c>
+      <c r="E1319" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1319" s="6">
+        <v>77.625</v>
+      </c>
+      <c r="G1319" s="6">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1320" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1320">
+        <v>0.7</v>
+      </c>
+      <c r="C1320" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1320">
+        <v>2</v>
+      </c>
+      <c r="E1320" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1320" s="6">
+        <v>81.125</v>
+      </c>
+      <c r="G1320" s="6">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1321" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1321">
+        <v>0.7</v>
+      </c>
+      <c r="C1321" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1321">
+        <v>5</v>
+      </c>
+      <c r="E1321" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1321" s="6">
+        <v>82.1</v>
+      </c>
+      <c r="G1321" s="6">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1322" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1322">
+        <v>0.7</v>
+      </c>
+      <c r="C1322" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1322">
+        <v>5</v>
+      </c>
+      <c r="E1322" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1322" s="6">
+        <v>74.125</v>
+      </c>
+      <c r="G1322" s="6">
+        <v>74.8</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1323" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1323">
+        <v>0.7</v>
+      </c>
+      <c r="C1323" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1323">
+        <v>8</v>
+      </c>
+      <c r="E1323" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1323" s="6">
+        <v>81.075000000000003</v>
+      </c>
+      <c r="G1323" s="6">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1324" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1324">
+        <v>0.7</v>
+      </c>
+      <c r="C1324" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1324">
+        <v>8</v>
+      </c>
+      <c r="E1324" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1324" s="6">
+        <v>64.875</v>
+      </c>
+      <c r="G1324" s="6">
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1325" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1325">
+        <v>0.7</v>
+      </c>
+      <c r="C1325" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1325">
+        <v>2</v>
+      </c>
+      <c r="E1325" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1325" s="6">
+        <v>80.075000000000003</v>
+      </c>
+      <c r="G1325" s="6">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1326" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1326">
+        <v>0.7</v>
+      </c>
+      <c r="C1326" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1326">
+        <v>2</v>
+      </c>
+      <c r="E1326" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1326" s="6">
+        <v>78.75</v>
+      </c>
+      <c r="G1326" s="6">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1327" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1327">
+        <v>0.7</v>
+      </c>
+      <c r="C1327" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1327">
+        <v>5</v>
+      </c>
+      <c r="E1327" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1327" s="6">
+        <v>79.525000000000006</v>
+      </c>
+      <c r="G1327" s="6">
+        <v>79.900000000000006</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1328" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1328">
+        <v>0.7</v>
+      </c>
+      <c r="C1328" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1328">
+        <v>5</v>
+      </c>
+      <c r="E1328" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1328" s="6">
+        <v>73</v>
+      </c>
+      <c r="G1328" s="6">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1329" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1329">
+        <v>0.7</v>
+      </c>
+      <c r="C1329" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1329">
+        <v>8</v>
+      </c>
+      <c r="E1329" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1329" s="6">
+        <v>79.174999999999997</v>
+      </c>
+      <c r="G1329" s="6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1330" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1330">
+        <v>0.7</v>
+      </c>
+      <c r="C1330" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1330">
+        <v>8</v>
+      </c>
+      <c r="E1330" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1330" s="6">
+        <v>65.275000000000006</v>
+      </c>
+      <c r="G1330" s="6">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1331" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1331">
+        <v>0.7</v>
+      </c>
+      <c r="C1331" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1331">
+        <v>2</v>
+      </c>
+      <c r="E1331" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1331" s="6">
+        <v>78.05</v>
+      </c>
+      <c r="G1331" s="6">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1332" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1332">
+        <v>0.7</v>
+      </c>
+      <c r="C1332" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1332">
+        <v>2</v>
+      </c>
+      <c r="E1332" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1332" s="6">
+        <v>81.699999999999903</v>
+      </c>
+      <c r="G1332" s="6">
+        <v>78.3</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1333" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1333">
+        <v>0.7</v>
+      </c>
+      <c r="C1333" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1333">
+        <v>5</v>
+      </c>
+      <c r="E1333" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1333" s="6">
+        <v>80.274999999999906</v>
+      </c>
+      <c r="G1333" s="6">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1334" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1334">
+        <v>0.7</v>
+      </c>
+      <c r="C1334" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1334">
+        <v>5</v>
+      </c>
+      <c r="E1334" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1334" s="6">
+        <v>70.849999999999994</v>
+      </c>
+      <c r="G1334" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1335" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1335">
+        <v>0.7</v>
+      </c>
+      <c r="C1335" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1335">
+        <v>8</v>
+      </c>
+      <c r="E1335" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1335" s="6">
+        <v>80.474999999999994</v>
+      </c>
+      <c r="G1335" s="6">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1336" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1336">
+        <v>0.7</v>
+      </c>
+      <c r="C1336" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1336">
+        <v>8</v>
+      </c>
+      <c r="E1336" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1336" s="6">
+        <v>66.025000000000006</v>
+      </c>
+      <c r="G1336" s="6">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1337" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1337">
+        <v>0.7</v>
+      </c>
+      <c r="C1337" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1337">
+        <v>2</v>
+      </c>
+      <c r="E1337" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1337" s="6">
+        <v>78.05</v>
+      </c>
+      <c r="G1337" s="6">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1338" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1338">
+        <v>0.7</v>
+      </c>
+      <c r="C1338" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1338">
+        <v>2</v>
+      </c>
+      <c r="E1338" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1338" s="6">
+        <v>81.349999999999994</v>
+      </c>
+      <c r="G1338" s="6">
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1339" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1339">
+        <v>0.7</v>
+      </c>
+      <c r="C1339" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1339">
+        <v>5</v>
+      </c>
+      <c r="E1339" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1339" s="6">
+        <v>78.474999999999994</v>
+      </c>
+      <c r="G1339" s="6">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1340" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1340">
+        <v>0.7</v>
+      </c>
+      <c r="C1340" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1340">
+        <v>5</v>
+      </c>
+      <c r="E1340" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1340" s="6">
+        <v>70.724999999999994</v>
+      </c>
+      <c r="G1340" s="6">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1341" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1341">
+        <v>0.7</v>
+      </c>
+      <c r="C1341" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1341">
+        <v>8</v>
+      </c>
+      <c r="E1341" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1341" s="6">
+        <v>78.55</v>
+      </c>
+      <c r="G1341" s="6">
+        <v>80.2</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1342" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1342">
+        <v>0.7</v>
+      </c>
+      <c r="C1342" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1342">
+        <v>8</v>
+      </c>
+      <c r="E1342" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1342" s="6">
+        <v>68.075000000000003</v>
+      </c>
+      <c r="G1342" s="6">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1343" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1343">
+        <v>0.8</v>
+      </c>
+      <c r="C1343" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1343">
+        <v>2</v>
+      </c>
+      <c r="E1343" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1343" s="6">
+        <v>79.7</v>
+      </c>
+      <c r="G1343" s="6">
+        <v>77.400000000000006</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1344" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1344">
+        <v>0.8</v>
+      </c>
+      <c r="C1344" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1344">
+        <v>2</v>
+      </c>
+      <c r="E1344" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1344" s="6">
+        <v>81.125</v>
+      </c>
+      <c r="G1344" s="6">
+        <v>77.7</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1345" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1345">
+        <v>0.8</v>
+      </c>
+      <c r="C1345" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1345">
+        <v>5</v>
+      </c>
+      <c r="E1345" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1345" s="6">
+        <v>82.224999999999994</v>
+      </c>
+      <c r="G1345" s="6">
+        <v>80.900000000000006</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1346" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1346">
+        <v>0.8</v>
+      </c>
+      <c r="C1346" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1346">
+        <v>5</v>
+      </c>
+      <c r="E1346" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1346" s="6">
+        <v>70.674999999999997</v>
+      </c>
+      <c r="G1346" s="6">
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1347" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1347">
+        <v>0.8</v>
+      </c>
+      <c r="C1347" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1347">
+        <v>8</v>
+      </c>
+      <c r="E1347" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1347" s="6">
+        <v>79.849999999999994</v>
+      </c>
+      <c r="G1347" s="6">
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1348" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1348">
+        <v>0.8</v>
+      </c>
+      <c r="C1348" s="6">
+        <v>40000</v>
+      </c>
+      <c r="D1348">
+        <v>8</v>
+      </c>
+      <c r="E1348" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1348" s="6">
+        <v>62.7</v>
+      </c>
+      <c r="G1348" s="6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1349" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1349">
+        <v>0.8</v>
+      </c>
+      <c r="C1349" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1349">
+        <v>2</v>
+      </c>
+      <c r="E1349" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1349" s="6">
+        <v>77.825000000000003</v>
+      </c>
+      <c r="G1349" s="6">
+        <v>74.599999999999994</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1350" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1350">
+        <v>0.8</v>
+      </c>
+      <c r="C1350" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1350">
+        <v>2</v>
+      </c>
+      <c r="E1350" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1350" s="6">
+        <v>80.7</v>
+      </c>
+      <c r="G1350" s="6">
+        <v>81.3</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1351" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1351">
+        <v>0.8</v>
+      </c>
+      <c r="C1351" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1351">
+        <v>5</v>
+      </c>
+      <c r="E1351" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1351" s="6">
+        <v>80.7</v>
+      </c>
+      <c r="G1351" s="6">
+        <v>81.599999999999994</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1352" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1352">
+        <v>0.8</v>
+      </c>
+      <c r="C1352" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1352">
+        <v>5</v>
+      </c>
+      <c r="E1352" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1352" s="6">
+        <v>70.55</v>
+      </c>
+      <c r="G1352" s="6">
+        <v>70.899999999999906</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1353" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1353">
+        <v>0.8</v>
+      </c>
+      <c r="C1353" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1353">
+        <v>8</v>
+      </c>
+      <c r="E1353" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1353" s="6">
+        <v>81.325000000000003</v>
+      </c>
+      <c r="G1353" s="6">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1354" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1354">
+        <v>0.8</v>
+      </c>
+      <c r="C1354" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D1354">
+        <v>8</v>
+      </c>
+      <c r="E1354" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1354" s="6">
+        <v>66.674999999999997</v>
+      </c>
+      <c r="G1354" s="6">
+        <v>61.1</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1355" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1355">
+        <v>0.8</v>
+      </c>
+      <c r="C1355" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1355">
+        <v>2</v>
+      </c>
+      <c r="E1355" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1355" s="6">
+        <v>78.375</v>
+      </c>
+      <c r="G1355" s="6">
+        <v>77.400000000000006</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1356" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1356">
+        <v>0.8</v>
+      </c>
+      <c r="C1356" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1356">
+        <v>2</v>
+      </c>
+      <c r="E1356" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1356" s="6">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="G1356" s="6">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1357" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1357">
+        <v>0.8</v>
+      </c>
+      <c r="C1357" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1357">
+        <v>5</v>
+      </c>
+      <c r="E1357" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1357" s="6">
+        <v>80.025000000000006</v>
+      </c>
+      <c r="G1357" s="6">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1358" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1358">
+        <v>0.8</v>
+      </c>
+      <c r="C1358" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1358">
+        <v>5</v>
+      </c>
+      <c r="E1358" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1358" s="6">
+        <v>70.775000000000006</v>
+      </c>
+      <c r="G1358" s="6">
+        <v>68.2</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1359" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1359">
+        <v>0.8</v>
+      </c>
+      <c r="C1359" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1359">
+        <v>8</v>
+      </c>
+      <c r="E1359" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1359" s="6">
+        <v>81.575000000000003</v>
+      </c>
+      <c r="G1359" s="6">
+        <v>81.699999999999903</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1360" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1360">
+        <v>0.8</v>
+      </c>
+      <c r="C1360" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D1360">
+        <v>8</v>
+      </c>
+      <c r="E1360" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1360" s="6">
+        <v>68.3</v>
+      </c>
+      <c r="G1360" s="6">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1361" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1361">
+        <v>0.8</v>
+      </c>
+      <c r="C1361" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1361">
+        <v>2</v>
+      </c>
+      <c r="E1361" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1361" s="6">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="G1361" s="6">
+        <v>76.900000000000006</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1362" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1362">
+        <v>0.8</v>
+      </c>
+      <c r="C1362" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1362">
+        <v>2</v>
+      </c>
+      <c r="E1362" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1362" s="6">
+        <v>80.825000000000003</v>
+      </c>
+      <c r="G1362" s="6">
+        <v>79.7</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1363" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1363">
+        <v>0.8</v>
+      </c>
+      <c r="C1363" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1363">
+        <v>5</v>
+      </c>
+      <c r="E1363" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1363" s="6">
+        <v>79</v>
+      </c>
+      <c r="G1363" s="6">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1364" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1364">
+        <v>0.8</v>
+      </c>
+      <c r="C1364" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1364">
+        <v>5</v>
+      </c>
+      <c r="E1364" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1364" s="6">
+        <v>68.95</v>
+      </c>
+      <c r="G1364" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1365" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1365">
+        <v>0.8</v>
+      </c>
+      <c r="C1365" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1365">
+        <v>8</v>
+      </c>
+      <c r="E1365" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1365" s="6">
+        <v>77.7</v>
+      </c>
+      <c r="G1365" s="6">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1366" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1366">
+        <v>0.8</v>
+      </c>
+      <c r="C1366" s="6">
+        <v>70000</v>
+      </c>
+      <c r="D1366">
+        <v>8</v>
+      </c>
+      <c r="E1366" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F1366" s="6">
+        <v>62.5</v>
+      </c>
+      <c r="G1366" s="6">
+        <v>64.7</v>
       </c>
     </row>
   </sheetData>
@@ -29008,7 +32137,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="G1:G1137 H1">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="num" val="8200"/>
@@ -29020,6 +32149,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1146:G1165">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1146:F1165">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -29031,7 +32172,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1146:F1165">
+  <conditionalFormatting sqref="F1284:F1366">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -29052,8 +32193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29061,32 +32202,32 @@
     <col min="1" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -29148,23 +32289,26 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>0.4</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="9">
         <v>40000</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
         <v>10000</v>
       </c>
-      <c r="F4" s="6">
-        <v>83.7</v>
-      </c>
-      <c r="G4" s="6">
-        <v>79.5</v>
+      <c r="F4" s="11">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.87</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.85</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -29190,6 +32334,9 @@
       <c r="G5" s="9">
         <v>666.26979522299996</v>
       </c>
+      <c r="H5" s="9">
+        <v>629</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -29214,6 +32361,9 @@
       <c r="G6" s="9">
         <v>22781.694873699998</v>
       </c>
+      <c r="H6">
+        <v>22068</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -29237,6 +32387,9 @@
       </c>
       <c r="G7" s="9">
         <v>14954.126240699999</v>
+      </c>
+      <c r="H7" s="9">
+        <v>14379</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -29244,16 +32397,54 @@
       <c r="A8" s="8">
         <v>6</v>
       </c>
+      <c r="B8" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>60000</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>25000</v>
+      </c>
+      <c r="F8" s="9">
+        <v>6288.0847741199996</v>
+      </c>
+      <c r="G8" s="9">
+        <v>114412.835913</v>
+      </c>
+      <c r="H8" s="9">
+        <v>108159</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="B9" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="9">
+        <v>80000</v>
+      </c>
+      <c r="D9" s="8">
+        <v>8</v>
+      </c>
+      <c r="E9" s="9">
+        <v>25000</v>
+      </c>
+      <c r="F9" s="9">
+        <v>3289.8766697299998</v>
+      </c>
+      <c r="G9" s="9">
+        <v>62713.338335300003</v>
+      </c>
+      <c r="H9" s="9">
+        <v>59030</v>
+      </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -29379,42 +32570,6 @@
       <c r="G27" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="8200"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="8200"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="8200"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
vFinal. Saved_state now gives >= 85% correct MNIST-classification
</commit_message>
<xml_diff>
--- a/module4/module4results.xlsx
+++ b/module4/module4results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="55">
   <si>
     <t>Learning rate0</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">5  0.6000000000000001 60000  8  25000  1236.25667421  15178.7971675  </t>
+  </si>
+  <si>
+    <t>Max_iterations</t>
   </si>
 </sst>
 </file>
@@ -32577,21 +32580,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="4" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -32608,16 +32611,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -32628,23 +32634,26 @@
         <v>80000</v>
       </c>
       <c r="D2" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="9">
         <v>25000</v>
       </c>
       <c r="F2" s="9">
+        <v>90000</v>
+      </c>
+      <c r="G2" s="9">
         <v>723.95567170100003</v>
       </c>
-      <c r="G2" s="9">
+      <c r="H2" s="9">
         <v>7962.6894577800003</v>
       </c>
-      <c r="H2" s="9">
+      <c r="I2" s="9">
         <v>7542</v>
       </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -32661,17 +32670,20 @@
         <v>25000</v>
       </c>
       <c r="F3" s="6">
+        <v>60000</v>
+      </c>
+      <c r="G3" s="6">
         <v>307.213486488</v>
       </c>
-      <c r="G3" s="6">
+      <c r="H3" s="6">
         <v>6337.3496746500005</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="6">
         <v>6110</v>
       </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -32688,17 +32700,20 @@
         <v>25000</v>
       </c>
       <c r="F4" s="9">
+        <v>60000</v>
+      </c>
+      <c r="G4" s="9">
         <v>17.8032640807</v>
       </c>
-      <c r="G4" s="9">
+      <c r="H4" s="9">
         <v>666.26979522299996</v>
       </c>
-      <c r="H4" s="9">
+      <c r="I4" s="9">
         <v>629</v>
       </c>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -32715,17 +32730,20 @@
         <v>25000</v>
       </c>
       <c r="F5" s="9">
+        <v>60000</v>
+      </c>
+      <c r="G5" s="9">
         <v>1305.98608375</v>
       </c>
-      <c r="G5" s="9">
+      <c r="H5" s="9">
         <v>22781.694873699998</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>22068</v>
       </c>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -32742,17 +32760,20 @@
         <v>25000</v>
       </c>
       <c r="F6" s="9">
+        <v>60000</v>
+      </c>
+      <c r="G6" s="9">
         <v>1112.0348659399999</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>14954.126240699999</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
         <v>14379</v>
       </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -32769,17 +32790,20 @@
         <v>25000</v>
       </c>
       <c r="F7" s="9">
+        <v>60000</v>
+      </c>
+      <c r="G7" s="9">
         <v>6288.0847741199996</v>
       </c>
-      <c r="G7" s="9">
+      <c r="H7" s="9">
         <v>114412.835913</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <v>108159</v>
       </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -32796,17 +32820,20 @@
         <v>25000</v>
       </c>
       <c r="F8" s="9">
+        <v>80000</v>
+      </c>
+      <c r="G8" s="9">
         <v>3289.8766697299998</v>
       </c>
-      <c r="G8" s="9">
+      <c r="H8" s="9">
         <v>62713.338335300003</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
         <v>59030</v>
       </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -32822,17 +32849,20 @@
       <c r="E9" s="6">
         <v>25000</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="9">
+        <v>60000</v>
+      </c>
+      <c r="G9" s="6">
         <v>24.5605055642</v>
       </c>
-      <c r="G9" s="6">
+      <c r="H9" s="6">
         <v>1240.45890003</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="6">
         <v>1211</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -32848,112 +32878,131 @@
       <c r="E10" s="9">
         <v>10000</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
+        <v>25000</v>
+      </c>
+      <c r="G10" s="11">
         <v>0.91500000000000004</v>
       </c>
-      <c r="G10" s="11">
+      <c r="H10" s="11">
         <v>0.87</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <v>0.85</v>
       </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>